<commit_message>
A new RTCurve with new data, 20mK need further scan
</commit_message>
<xml_diff>
--- a/output/RTCurve.xlsx
+++ b/output/RTCurve.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\File\Particle_Physics\Experiments\0vbb\Electronics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\File\Particle_Physics\Experiments\0vbb\Electronics\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47892F19-EAEB-4CD0-997B-17D1286B5A5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF80314-0676-4ECD-9B78-9D9CF169BD3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
     <sheet name="buyaokan" sheetId="4" r:id="rId3"/>
+    <sheet name="Final" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="9">
   <si>
     <t>Temperature</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -46,6 +47,22 @@
   </si>
   <si>
     <t>T^(-0.5)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Temp Min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Temp Max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Temperature(Sample)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Temp (MXC)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2142,6 +2159,765 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Final!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3x3NTD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Final!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>7.0675349274021944</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7115605521402424</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7807331301608</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1292169078594849</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0065754482492739</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.8923304344598968</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.0003125292999275</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.4725832356883011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1628312040684214</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Final!$F$2:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>33200000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19700000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3510000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>682200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>535200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>388200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>525800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>142200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5775</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BC3B-4610-A36B-F0E2CDE94945}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Final!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3x1NTD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Final!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>7.0675349274021944</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7115605521402424</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7807331301608</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1292169078594849</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0065754482492739</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.8923304344598968</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.0003125292999275</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.4725832356883011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1628312040684214</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Final!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>32200000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20900000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4460000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1761500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1437000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1112500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1354900</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>419550</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21981.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-BC3B-4610-A36B-F0E2CDE94945}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Final!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>19T20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Final!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>7.0675349274021944</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7115605521402424</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7807331301608</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1292169078594849</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0065754482492739</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.8923304344598968</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.0003125292999275</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.4725832356883011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1628312040684214</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Final!$H$2:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>26300000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14360000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2590000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>526900</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>425100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>323300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>407600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>112530</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4942</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-BC3B-4610-A36B-F0E2CDE94945}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1790123072"/>
+        <c:axId val="1782958800"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1790123072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="3"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>T^(-0.5)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00_);[Red]\(#,##0.00\)" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1782958800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.25"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1782958800"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>R_NTD</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-CN"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>[Ω]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1790123072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2262,6 +3038,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3355,6 +4171,582 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="250">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="250">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4035,6 +5427,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{015EE797-5697-4348-876A-56F0069B3C85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>282817</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>119912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>410309</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>58615</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60425367-42A5-4CEA-A37A-6EFBAFBA0D1D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4413,8 +5848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D7640E-DE5C-4A77-9437-80077CEF9058}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4571,7 +6006,7 @@
         <v>2.0420000000000001E-2</v>
       </c>
       <c r="B2" s="1">
-        <f>POWER(A2,-0.5)</f>
+        <f t="shared" ref="B2:B7" si="0">POWER(A2,-0.5)</f>
         <v>6.9979708826234095</v>
       </c>
       <c r="C2" s="1">
@@ -4589,7 +6024,7 @@
         <v>2.8094999999999998E-2</v>
       </c>
       <c r="B3" s="1">
-        <f>POWER(A3,-0.5)</f>
+        <f t="shared" si="0"/>
         <v>5.9660306719794711</v>
       </c>
       <c r="C3" s="1">
@@ -4607,7 +6042,7 @@
         <v>3.5860000000000003E-2</v>
       </c>
       <c r="B4" s="1">
-        <f>POWER(A4,-0.5)</f>
+        <f t="shared" si="0"/>
         <v>5.2807408765477799</v>
       </c>
       <c r="C4" s="1">
@@ -4625,7 +6060,7 @@
         <v>3.7545000000000002E-2</v>
       </c>
       <c r="B5" s="1">
-        <f>POWER(A5,-0.5)</f>
+        <f t="shared" si="0"/>
         <v>5.1608821940286429</v>
       </c>
       <c r="C5" s="1">
@@ -4643,7 +6078,7 @@
         <v>3.9230000000000001E-2</v>
       </c>
       <c r="B6" s="1">
-        <f>POWER(A6,-0.5)</f>
+        <f t="shared" si="0"/>
         <v>5.0488311415611795</v>
       </c>
       <c r="C6" s="1">
@@ -4661,7 +6096,7 @@
         <v>295</v>
       </c>
       <c r="B7" s="1">
-        <f>POWER(A7,-0.5)</f>
+        <f t="shared" si="0"/>
         <v>5.8222250973958202E-2</v>
       </c>
       <c r="C7" s="1">
@@ -4672,6 +6107,308 @@
       </c>
       <c r="E7" s="1">
         <v>11.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3DC8920-43B3-479D-AA61-3FC0F10AF091}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>19.89</v>
+      </c>
+      <c r="B2">
+        <v>20.149999999999999</v>
+      </c>
+      <c r="C2" s="1">
+        <f>(A2+B2)/2/1000</f>
+        <v>2.002E-2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="E2" s="1">
+        <f t="shared" ref="E2:E10" si="0">POWER(C2,-0.5)</f>
+        <v>7.0675349274021944</v>
+      </c>
+      <c r="F2" s="1">
+        <v>33200000</v>
+      </c>
+      <c r="G2" s="1">
+        <v>32200000</v>
+      </c>
+      <c r="H2" s="1">
+        <v>26300000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>21.52</v>
+      </c>
+      <c r="B3">
+        <v>22.88</v>
+      </c>
+      <c r="C3" s="1">
+        <f>(A3+B3)/2/1000</f>
+        <v>2.2200000000000001E-2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2.0420000000000001E-2</v>
+      </c>
+      <c r="E3" s="1">
+        <f>POWER(C3,-0.5)</f>
+        <v>6.7115605521402424</v>
+      </c>
+      <c r="F3" s="1">
+        <v>19700000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>20900000</v>
+      </c>
+      <c r="H3" s="1">
+        <v>14360000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>28.33</v>
+      </c>
+      <c r="B4">
+        <v>31.52</v>
+      </c>
+      <c r="C4" s="1">
+        <f>(A4+B4)/2/1000</f>
+        <v>2.9924999999999997E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2.8094999999999998E-2</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>5.7807331301608</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3510000</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4460000</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2590000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>38.01</v>
+      </c>
+      <c r="B5">
+        <v>38.01</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" ref="C5:C10" si="1">(A5+B5)/2/1000</f>
+        <v>3.8009999999999995E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3.5860000000000003E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>5.1292169078594849</v>
+      </c>
+      <c r="F5" s="1">
+        <v>682200</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1761500</v>
+      </c>
+      <c r="H5" s="1">
+        <v>526900</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>38.01</v>
+      </c>
+      <c r="B6">
+        <v>41.78</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="1"/>
+        <v>3.9894999999999993E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3.7545000000000002E-2</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>5.0065754482492739</v>
+      </c>
+      <c r="F6" s="1">
+        <v>535200</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1437000</v>
+      </c>
+      <c r="H6" s="1">
+        <v>425100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>41.78</v>
+      </c>
+      <c r="B7">
+        <v>41.78</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="1"/>
+        <v>4.1779999999999998E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3.9230000000000001E-2</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>4.8923304344598968</v>
+      </c>
+      <c r="F7" s="1">
+        <v>388200</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1112500</v>
+      </c>
+      <c r="H7" s="1">
+        <v>323300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>39.9</v>
+      </c>
+      <c r="B8">
+        <v>40.090000000000003</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="1"/>
+        <v>3.9995000000000003E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>5.0003125292999275</v>
+      </c>
+      <c r="F8" s="1">
+        <v>525800</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1354900</v>
+      </c>
+      <c r="H8" s="1">
+        <v>407600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>49.94</v>
+      </c>
+      <c r="B9">
+        <v>50.04</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="1"/>
+        <v>4.9989999999999993E-2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>4.4725832356883011</v>
+      </c>
+      <c r="F9" s="1">
+        <v>142200</v>
+      </c>
+      <c r="G9" s="1">
+        <v>419550</v>
+      </c>
+      <c r="H9" s="1">
+        <v>112530</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>99.81</v>
+      </c>
+      <c r="B10">
+        <v>100.12</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="1"/>
+        <v>9.9964999999999998E-2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>3.1628312040684214</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5775</v>
+      </c>
+      <c r="G10" s="1">
+        <v>21981.3</v>
+      </c>
+      <c r="H10" s="1">
+        <v>4942</v>
       </c>
     </row>
   </sheetData>

</xml_diff>